<commit_message>
add statement to close the properties file
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="560" windowWidth="24220" windowHeight="14980" tabRatio="971" activeTab="11"/>
+    <workbookView xWindow="600" yWindow="560" windowWidth="24220" windowHeight="14980" tabRatio="971" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Home Page" sheetId="13" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="126">
   <si>
     <t>Test Case No.</t>
   </si>
@@ -357,13 +357,7 @@
     <t>Not tried to run the test as not sure whether I can use the same password again</t>
   </si>
   <si>
-    <t>Add assertion</t>
-  </si>
-  <si>
     <t>Validate Name field for only upper case characters</t>
-  </si>
-  <si>
-    <t>Add Assertions</t>
   </si>
   <si>
     <t>Query for existing record using Branch Code</t>
@@ -1364,10 +1358,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>91</v>
@@ -1388,7 +1382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -1422,7 +1416,7 @@
         <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>91</v>
@@ -1434,16 +1428,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1451,16 +1445,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1471,7 +1465,7 @@
         <v>83</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>91</v>
@@ -1483,10 +1477,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>91</v>
@@ -1965,7 +1959,7 @@
         <v>91</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2087,7 +2081,7 @@
         <v>91</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="32">
@@ -2185,7 +2179,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>15</v>
@@ -2209,7 +2203,7 @@
         <v>91</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2226,7 +2220,7 @@
         <v>91</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -2368,7 +2362,7 @@
         <v>41</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>91</v>
@@ -2380,10 +2374,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>91</v>
@@ -2403,10 +2397,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -2415,7 +2409,7 @@
     <col min="3" max="3" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2432,7 +2426,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:5">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2445,7 +2439,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:5">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2460,7 +2454,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:5">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2475,7 +2469,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:5">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2489,11 +2483,8 @@
         <v>91</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2507,11 +2498,8 @@
         <v>91</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2525,11 +2513,8 @@
         <v>91</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2544,7 +2529,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:5">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2559,7 +2544,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:5">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2574,7 +2559,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:5">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2589,7 +2574,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:5">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2604,7 +2589,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:5">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2618,11 +2603,8 @@
         <v>91</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2636,11 +2618,8 @@
         <v>91</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2655,7 +2634,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:5">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2670,7 +2649,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:5">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2685,7 +2664,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:5">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2699,11 +2678,8 @@
         <v>91</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2717,11 +2693,8 @@
         <v>91</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2735,11 +2708,8 @@
         <v>91</v>
       </c>
       <c r="E20" s="2"/>
-      <c r="F20" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2754,7 +2724,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:5">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2769,7 +2739,7 @@
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:5">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2783,11 +2753,8 @@
         <v>91</v>
       </c>
       <c r="E23" s="2"/>
-      <c r="F23" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2802,7 +2769,7 @@
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:5">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -2816,11 +2783,8 @@
         <v>91</v>
       </c>
       <c r="E25" s="2"/>
-      <c r="F25" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -3177,10 +3141,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>91</v>
@@ -3237,7 +3201,7 @@
         <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>91</v>
@@ -3249,10 +3213,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>91</v>
@@ -3264,10 +3228,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>91</v>
@@ -3282,7 +3246,7 @@
         <v>83</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>91</v>
@@ -3294,10 +3258,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>91</v>
@@ -3316,10 +3280,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -3328,7 +3292,7 @@
     <col min="3" max="3" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3345,7 +3309,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:5">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -3358,7 +3322,7 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:5">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -3373,7 +3337,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:5">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3387,11 +3351,8 @@
         <v>91</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3405,11 +3366,8 @@
         <v>91</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -3424,7 +3382,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:5">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -3439,7 +3397,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:5">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -3454,7 +3412,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:5">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -3469,7 +3427,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:5">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -3484,7 +3442,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:5">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -3498,16 +3456,13 @@
         <v>91</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>14</v>
@@ -3516,11 +3471,8 @@
         <v>91</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -3534,11 +3486,8 @@
         <v>91</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="3">
         <v>13</v>
       </c>

</xml_diff>